<commit_message>
updated release and test plan
</commit_message>
<xml_diff>
--- a/Documents/burndown charts.xlsx
+++ b/Documents/burndown charts.xlsx
@@ -11,6 +11,9 @@
     <sheet state="visible" name="week 8" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="sprint2" sheetId="7" r:id="rId9"/>
     <sheet state="visible" name="Release1" sheetId="8" r:id="rId10"/>
+    <sheet state="visible" name="week9" sheetId="9" r:id="rId11"/>
+    <sheet state="visible" name="week10" sheetId="10" r:id="rId12"/>
+    <sheet state="visible" name="sprint3" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -18,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="60">
   <si>
     <t>Week 5</t>
   </si>
@@ -65,9 +68,36 @@
     <t>TOTAL W5</t>
   </si>
   <si>
+    <t>Total hours</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>Day 4</t>
+  </si>
+  <si>
+    <t>Day 5</t>
+  </si>
+  <si>
+    <t>Day 6</t>
+  </si>
+  <si>
+    <t>Day 7</t>
+  </si>
+  <si>
     <t>Week 6</t>
   </si>
   <si>
+    <t>Expected time use</t>
+  </si>
+  <si>
     <t>TOTAL W6</t>
   </si>
   <si>
@@ -77,46 +107,25 @@
     <t>TOTAL W7</t>
   </si>
   <si>
-    <t>Total hours</t>
-  </si>
-  <si>
-    <t>Day 1</t>
+    <t>Actual time spent</t>
   </si>
   <si>
     <t>Week 8</t>
   </si>
   <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>Expected time use</t>
+    <t>This means that we are on schedule, but since Jack's does not contribute we have worked 8 hours overtime</t>
   </si>
   <si>
     <t>TOTAL W8</t>
   </si>
   <si>
-    <t>Actual time spent</t>
+    <t>Week 9</t>
   </si>
   <si>
     <t>This means that we are 4 hours behind schedule, but since Jack's does not contribute we have worked 4 hours overtime</t>
   </si>
   <si>
-    <t>This means that we are on schedule, but since Jack's does not contribute we have worked 8 hours overtime</t>
+    <t>Week 10</t>
   </si>
   <si>
     <t>Day 8</t>
@@ -442,11 +451,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="994305101"/>
-        <c:axId val="773027955"/>
+        <c:axId val="1189944593"/>
+        <c:axId val="1584758102"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="994305101"/>
+        <c:axId val="1189944593"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,10 +487,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773027955"/>
+        <c:crossAx val="1584758102"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="773027955"/>
+        <c:axId val="1584758102"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +538,171 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="994305101"/>
+        <c:crossAx val="1189944593"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Actual time spent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sprint3!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>sprint3!$B$1:$P$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sprint3!$B$2:$P$2</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sprint3!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>sprint3!$B$1:$P$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sprint3!$B$3:$P$3</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="959290196"/>
+        <c:axId val="1866971893"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="959290196"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1866971893"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1866971893"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Actual time spent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="959290196"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -627,11 +800,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1473678165"/>
-        <c:axId val="1845541906"/>
+        <c:axId val="921603040"/>
+        <c:axId val="241197687"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1473678165"/>
+        <c:axId val="921603040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,10 +819,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1845541906"/>
+        <c:crossAx val="241197687"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1845541906"/>
+        <c:axId val="241197687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,7 +870,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1473678165"/>
+        <c:crossAx val="921603040"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -795,11 +968,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="972606193"/>
-        <c:axId val="1192580105"/>
+        <c:axId val="1234205557"/>
+        <c:axId val="610940904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="972606193"/>
+        <c:axId val="1234205557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,10 +1004,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1192580105"/>
+        <c:crossAx val="610940904"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1192580105"/>
+        <c:axId val="610940904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +1055,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972606193"/>
+        <c:crossAx val="1234205557"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -980,11 +1153,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="646247325"/>
-        <c:axId val="78915375"/>
+        <c:axId val="1339391126"/>
+        <c:axId val="469400847"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="646247325"/>
+        <c:axId val="1339391126"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,10 +1189,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78915375"/>
+        <c:crossAx val="469400847"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78915375"/>
+        <c:axId val="469400847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1240,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="646247325"/>
+        <c:crossAx val="1339391126"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1165,11 +1338,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2142681181"/>
-        <c:axId val="1694275264"/>
+        <c:axId val="1551252474"/>
+        <c:axId val="2038886139"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142681181"/>
+        <c:axId val="1551252474"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,10 +1374,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1694275264"/>
+        <c:crossAx val="2038886139"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1694275264"/>
+        <c:axId val="2038886139"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1425,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142681181"/>
+        <c:crossAx val="1551252474"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1350,11 +1523,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="417454544"/>
-        <c:axId val="1917654117"/>
+        <c:axId val="2043356695"/>
+        <c:axId val="740894752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="417454544"/>
+        <c:axId val="2043356695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1386,10 +1559,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1917654117"/>
+        <c:crossAx val="740894752"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1917654117"/>
+        <c:axId val="740894752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,7 +1610,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417454544"/>
+        <c:crossAx val="2043356695"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1535,11 +1708,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="339425843"/>
-        <c:axId val="1962828192"/>
+        <c:axId val="2084169899"/>
+        <c:axId val="881262488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="339425843"/>
+        <c:axId val="2084169899"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,10 +1727,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1962828192"/>
+        <c:crossAx val="881262488"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1962828192"/>
+        <c:axId val="881262488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,7 +1761,335 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339425843"/>
+        <c:crossAx val="2084169899"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Actual time spent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>week9!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>week9!$B$1:$I$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>week9!$B$2:$I$2</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>week9!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>week9!$B$1:$I$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>week9!$B$3:$I$3</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="516428799"/>
+        <c:axId val="1511072594"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="516428799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1511072594"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1511072594"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Actual time spent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="516428799"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Actual time spent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>week10!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>week10!$B$1:$I$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>week10!$B$2:$I$2</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>week10!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>week10!$B$1:$I$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>week10!$B$3:$I$3</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1246916280"/>
+        <c:axId val="116268426"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1246916280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="116268426"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="116268426"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Actual time spent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1246916280"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1601,6 +2102,76 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 8" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 9" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1620,7 +2191,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1655,7 +2226,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1725,7 +2296,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1760,7 +2331,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1795,7 +2366,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1848,6 +2419,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -1916,7 +2522,7 @@
         <v>1.0</v>
       </c>
       <c r="I3" s="12"/>
-      <c r="J3" s="13" t="str">
+      <c r="J3" s="13">
         <f t="shared" ref="J3:J7" si="1">sum(C3:I3)</f>
         <v>6</v>
       </c>
@@ -1939,7 +2545,7 @@
       <c r="I4" s="12">
         <v>2.0</v>
       </c>
-      <c r="J4" s="13" t="str">
+      <c r="J4" s="13">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -1958,7 +2564,7 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="11"/>
-      <c r="J5" s="13" t="str">
+      <c r="J5" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1983,7 +2589,7 @@
       <c r="I6" s="12">
         <v>5.0</v>
       </c>
-      <c r="J6" s="13" t="str">
+      <c r="J6" s="13">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -1992,39 +2598,39 @@
       <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17" t="str">
+      <c r="B7" s="17">
         <f t="shared" ref="B7:I7" si="2">SUM(B3:B6)</f>
         <v>32</v>
       </c>
-      <c r="C7" s="17" t="str">
+      <c r="C7" s="17">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D7" s="17" t="str">
+      <c r="D7" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E7" s="17" t="str">
+      <c r="E7" s="17">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F7" s="17" t="str">
+      <c r="F7" s="17">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="G7" s="17" t="str">
+      <c r="G7" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H7" s="17" t="str">
+      <c r="H7" s="17">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="I7" s="17" t="str">
+      <c r="I7" s="17">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="J7" s="18" t="str">
+      <c r="J7" s="18">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -2051,7 +2657,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2110,7 +2716,7 @@
       <c r="I12" s="12">
         <v>2.0</v>
       </c>
-      <c r="J12" s="13" t="str">
+      <c r="J12" s="13">
         <f t="shared" ref="J12:J16" si="3">sum(C12:I12)</f>
         <v>9</v>
       </c>
@@ -2139,7 +2745,7 @@
       <c r="I13" s="12">
         <v>2.0</v>
       </c>
-      <c r="J13" s="13" t="str">
+      <c r="J13" s="13">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
@@ -2157,7 +2763,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
-      <c r="J14" s="13" t="str">
+      <c r="J14" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2181,48 +2787,48 @@
         <v>2.0</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="J15" s="13" t="str">
+      <c r="J15" s="13">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="17" t="str">
+        <v>25</v>
+      </c>
+      <c r="B16" s="17">
         <f t="shared" ref="B16:I16" si="4">SUM(B12:B15)</f>
         <v>32</v>
       </c>
-      <c r="C16" s="17" t="str">
+      <c r="C16" s="17">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="D16" s="17" t="str">
+      <c r="D16" s="17">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="E16" s="17" t="str">
+      <c r="E16" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F16" s="17" t="str">
+      <c r="F16" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G16" s="17" t="str">
+      <c r="G16" s="17">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="H16" s="17" t="str">
+      <c r="H16" s="17">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I16" s="17" t="str">
+      <c r="I16" s="17">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="J16" s="18" t="str">
+      <c r="J16" s="18">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
@@ -2239,7 +2845,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2301,7 +2907,7 @@
       <c r="I20" s="12">
         <v>2.0</v>
       </c>
-      <c r="J20" s="13" t="str">
+      <c r="J20" s="13">
         <f t="shared" ref="J20:J24" si="5">sum(C20:I20)</f>
         <v>7</v>
       </c>
@@ -2328,7 +2934,7 @@
         <v>3.0</v>
       </c>
       <c r="I21" s="12"/>
-      <c r="J21" s="13" t="str">
+      <c r="J21" s="13">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
@@ -2346,7 +2952,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="11"/>
       <c r="H22" s="12"/>
-      <c r="J22" s="13" t="str">
+      <c r="J22" s="13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2370,55 +2976,55 @@
       <c r="H23" s="12">
         <v>3.0</v>
       </c>
-      <c r="J23" s="13" t="str">
+      <c r="J23" s="13">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="17" t="str">
+        <v>27</v>
+      </c>
+      <c r="B24" s="17">
         <f t="shared" ref="B24:I24" si="6">SUM(B20:B23)</f>
         <v>32</v>
       </c>
-      <c r="C24" s="17" t="str">
+      <c r="C24" s="17">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="D24" s="17" t="str">
+      <c r="D24" s="17">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="E24" s="17" t="str">
+      <c r="E24" s="17">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="F24" s="17" t="str">
+      <c r="F24" s="17">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="G24" s="17" t="str">
+      <c r="G24" s="17">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="H24" s="17" t="str">
+      <c r="H24" s="17">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="I24" s="17" t="str">
+      <c r="I24" s="17">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="J24" s="18" t="str">
+      <c r="J24" s="18">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2477,7 +3083,7 @@
       <c r="I28" s="12">
         <v>5.0</v>
       </c>
-      <c r="J28" s="13" t="str">
+      <c r="J28" s="13">
         <f t="shared" ref="J28:J32" si="7">sum(C28:I28)</f>
         <v>9</v>
       </c>
@@ -2502,7 +3108,7 @@
       <c r="I29" s="12">
         <v>5.0</v>
       </c>
-      <c r="J29" s="13" t="str">
+      <c r="J29" s="13">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
@@ -2520,7 +3126,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
       <c r="H30" s="12"/>
-      <c r="J30" s="13" t="str">
+      <c r="J30" s="13">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2547,54 +3153,722 @@
       <c r="I31" s="12">
         <v>4.0</v>
       </c>
-      <c r="J31" s="13" t="str">
+      <c r="J31" s="13">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="17" t="str">
+        <v>31</v>
+      </c>
+      <c r="B32" s="17">
         <f t="shared" ref="B32:I32" si="8">SUM(B28:B31)</f>
         <v>32</v>
       </c>
-      <c r="C32" s="17" t="str">
+      <c r="C32" s="17">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="D32" s="17" t="str">
+      <c r="D32" s="17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E32" s="17" t="str">
+      <c r="E32" s="17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F32" s="17" t="str">
+      <c r="F32" s="17">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="G32" s="17" t="str">
+      <c r="G32" s="17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H32" s="17" t="str">
+      <c r="H32" s="17">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="I32" s="17" t="str">
+      <c r="I32" s="17">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="J32" s="18" t="str">
+      <c r="J32" s="18">
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="12"/>
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C36" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I36" s="12"/>
+      <c r="J36" s="13">
+        <f t="shared" ref="J36:J40" si="9">sum(C36:I36)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C37" s="9">
+        <v>6.0</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11">
+        <v>4.0</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I37" s="12"/>
+      <c r="J37" s="13">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="12"/>
+      <c r="J38" s="13">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C39" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="J39" s="13">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="17">
+        <f t="shared" ref="B40:I40" si="10">SUM(B36:B39)</f>
+        <v>24</v>
+      </c>
+      <c r="C40" s="17">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="D40" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="17">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="F40" s="17">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="G40" s="17">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H40" s="17">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="I40" s="17">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="J40" s="18">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="I44" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J44" s="13">
+        <f t="shared" ref="J44:J48" si="11">sum(C44:I44)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9">
+        <v>7.0</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="J45" s="13">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="12"/>
+      <c r="J46" s="13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="G47" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="13">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="17">
+        <f t="shared" ref="B48:I48" si="12">SUM(B44:B47)</f>
+        <v>24</v>
+      </c>
+      <c r="C48" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="17">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="E48" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="17">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="G48" s="17">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="H48" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="17">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="J48" s="18">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.43"/>
+    <col customWidth="1" min="2" max="2" width="12.0"/>
+    <col customWidth="1" min="3" max="4" width="10.29"/>
+    <col customWidth="1" min="5" max="5" width="10.57"/>
+    <col customWidth="1" min="6" max="8" width="10.0"/>
+    <col customWidth="1" min="9" max="9" width="9.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9"/>
+      <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
+        <f>SUM(hours!B44:B47)</f>
+        <v>24</v>
+      </c>
+      <c r="C2" s="24">
+        <f>(B2/7)*6</f>
+        <v>20.57142857</v>
+      </c>
+      <c r="D2" s="24">
+        <f>(B2/7)*5</f>
+        <v>17.14285714</v>
+      </c>
+      <c r="E2" s="24">
+        <f>(B2/7)*4</f>
+        <v>13.71428571</v>
+      </c>
+      <c r="F2" s="24">
+        <f>(B2/7)*3</f>
+        <v>10.28571429</v>
+      </c>
+      <c r="G2" s="24">
+        <f>(B2/7)*2</f>
+        <v>6.857142857</v>
+      </c>
+      <c r="H2" s="24">
+        <f>(B2/7)*1</f>
+        <v>3.428571429</v>
+      </c>
+      <c r="I2" s="24">
+        <f>(B2/7)*0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
+        <f>B2</f>
+        <v>24</v>
+      </c>
+      <c r="C3" s="24">
+        <f>B3-SUM(hours!C44:C47)</f>
+        <v>24</v>
+      </c>
+      <c r="D3" s="24">
+        <f>C3-SUM(hours!D44:D47)</f>
+        <v>14</v>
+      </c>
+      <c r="E3" s="24">
+        <f>D3-SUM(hours!E44:E47)</f>
+        <v>14</v>
+      </c>
+      <c r="F3" s="24">
+        <f>E3-SUM(hours!F44:F47)</f>
+        <v>12</v>
+      </c>
+      <c r="G3" s="24">
+        <f>F3-SUM(hours!G44:G47)</f>
+        <v>7</v>
+      </c>
+      <c r="H3" s="24">
+        <f>G3-SUM(hours!H44:H47)</f>
+        <v>7</v>
+      </c>
+      <c r="I3" s="24">
+        <f>H3-SUM(hours!I44:I47)</f>
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="3" max="3" width="9.71"/>
+    <col customWidth="1" min="4" max="4" width="10.29"/>
+    <col customWidth="1" min="5" max="5" width="10.0"/>
+    <col customWidth="1" min="6" max="6" width="10.57"/>
+    <col customWidth="1" min="7" max="7" width="9.71"/>
+    <col customWidth="1" min="8" max="8" width="10.29"/>
+    <col customWidth="1" min="9" max="9" width="10.57"/>
+    <col customWidth="1" min="10" max="10" width="8.57"/>
+    <col customWidth="1" min="11" max="11" width="7.14"/>
+    <col customWidth="1" min="12" max="12" width="8.57"/>
+    <col customWidth="1" min="13" max="13" width="8.29"/>
+    <col customWidth="1" min="14" max="14" width="9.14"/>
+    <col customWidth="1" min="15" max="15" width="8.0"/>
+    <col customWidth="1" min="16" max="16" width="8.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9"/>
+      <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
+        <f>24+24</f>
+        <v>48</v>
+      </c>
+      <c r="C2" s="24">
+        <f>(B2/14)*13</f>
+        <v>44.57142857</v>
+      </c>
+      <c r="D2" s="24">
+        <f>(B2/14)*12</f>
+        <v>41.14285714</v>
+      </c>
+      <c r="E2" s="24">
+        <f>(B2/14)*11</f>
+        <v>37.71428571</v>
+      </c>
+      <c r="F2" s="24">
+        <f>(B2/14)*10</f>
+        <v>34.28571429</v>
+      </c>
+      <c r="G2" s="24">
+        <f>(B2/14)*9</f>
+        <v>30.85714286</v>
+      </c>
+      <c r="H2" s="24">
+        <f>(B2/14)*8</f>
+        <v>27.42857143</v>
+      </c>
+      <c r="I2" s="24">
+        <f>(B2/14)*7</f>
+        <v>24</v>
+      </c>
+      <c r="J2" s="24">
+        <f>(B2/14)*6</f>
+        <v>20.57142857</v>
+      </c>
+      <c r="K2" s="24">
+        <f>(B2/14)*5</f>
+        <v>17.14285714</v>
+      </c>
+      <c r="L2" s="24">
+        <f>(B2/14)*4</f>
+        <v>13.71428571</v>
+      </c>
+      <c r="M2" s="24">
+        <f>(B2/14)*3</f>
+        <v>10.28571429</v>
+      </c>
+      <c r="N2" s="24">
+        <f>(B2/14)*2</f>
+        <v>6.857142857</v>
+      </c>
+      <c r="O2" s="24">
+        <f>(B2/14)*1</f>
+        <v>3.428571429</v>
+      </c>
+      <c r="P2" s="24">
+        <f>(B2/14)*0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
+        <f>B2</f>
+        <v>48</v>
+      </c>
+      <c r="C3" s="24">
+        <f>B3-SUM(hours!C36:C39)</f>
+        <v>37</v>
+      </c>
+      <c r="D3" s="24">
+        <f>C3-SUM(hours!D36:D39)</f>
+        <v>37</v>
+      </c>
+      <c r="E3" s="24">
+        <f>D3-SUM(hours!E36:E39)</f>
+        <v>35</v>
+      </c>
+      <c r="F3" s="24">
+        <f>E3-SUM(hours!F36:F39)</f>
+        <v>31</v>
+      </c>
+      <c r="G3" s="24">
+        <f>F3-SUM(hours!G36:G39)</f>
+        <v>29</v>
+      </c>
+      <c r="H3" s="24">
+        <f>G3-SUM(hours!H36:H39)</f>
+        <v>25</v>
+      </c>
+      <c r="I3" s="24">
+        <f>H3-SUM(hours!I36:I39)</f>
+        <v>23</v>
+      </c>
+      <c r="J3" s="26">
+        <f>I3-SUM(hours!C44:C47)</f>
+        <v>23</v>
+      </c>
+      <c r="K3" s="26">
+        <f>J3-SUM(hours!D44:D47)</f>
+        <v>13</v>
+      </c>
+      <c r="L3" s="26">
+        <f>K3-SUM(hours!E44:E47)</f>
+        <v>13</v>
+      </c>
+      <c r="M3" s="26">
+        <f>L3-SUM(hours!F44:F47)</f>
+        <v>11</v>
+      </c>
+      <c r="N3" s="26">
+        <f>M3-SUM(hours!G44:G47)</f>
+        <v>6</v>
+      </c>
+      <c r="O3" s="26">
+        <f>N3-SUM(hours!H44:H47)</f>
+        <v>6</v>
+      </c>
+      <c r="P3" s="26">
+        <f>O3-SUM(hours!I44:I47)</f>
+        <v>-2</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2623,105 +3897,105 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="24" t="str">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <f>SUM(hours!B3:B6)</f>
-        <v>32.00</v>
-      </c>
-      <c r="C2" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="C2" s="24">
         <f>(B2/7)*6</f>
-        <v>27.43</v>
-      </c>
-      <c r="D2" s="24" t="str">
+        <v>27.42857143</v>
+      </c>
+      <c r="D2" s="24">
         <f>(B2/7)*5</f>
-        <v>22.86</v>
-      </c>
-      <c r="E2" s="24" t="str">
+        <v>22.85714286</v>
+      </c>
+      <c r="E2" s="24">
         <f>(B2/7)*4</f>
-        <v>18.29</v>
-      </c>
-      <c r="F2" s="24" t="str">
+        <v>18.28571429</v>
+      </c>
+      <c r="F2" s="24">
         <f>(B2/7)*3</f>
-        <v>13.71</v>
-      </c>
-      <c r="G2" s="24" t="str">
+        <v>13.71428571</v>
+      </c>
+      <c r="G2" s="24">
         <f>(B2/7)*2</f>
-        <v>9.14</v>
-      </c>
-      <c r="H2" s="24" t="str">
+        <v>9.142857143</v>
+      </c>
+      <c r="H2" s="24">
         <f>(B2/7)*1</f>
-        <v>4.57</v>
-      </c>
-      <c r="I2" s="24" t="str">
+        <v>4.571428571</v>
+      </c>
+      <c r="I2" s="24">
         <f>(B2/7)*0</f>
-        <v>0.00</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="24" t="str">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
         <f>B2</f>
-        <v>32.00</v>
-      </c>
-      <c r="C3" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="C3" s="24">
         <f>B3-SUM(hours!C3:C6)</f>
-        <v>22.00</v>
-      </c>
-      <c r="D3" s="24" t="str">
+        <v>22</v>
+      </c>
+      <c r="D3" s="24">
         <f>C3-SUM(hours!D3:D6)</f>
-        <v>22.00</v>
-      </c>
-      <c r="E3" s="24" t="str">
+        <v>22</v>
+      </c>
+      <c r="E3" s="24">
         <f>D3-SUM(hours!E3:E6)</f>
-        <v>19.00</v>
-      </c>
-      <c r="F3" s="24" t="str">
+        <v>19</v>
+      </c>
+      <c r="F3" s="24">
         <f>E3-SUM(hours!F3:F6)</f>
-        <v>17.00</v>
-      </c>
-      <c r="G3" s="24" t="str">
+        <v>17</v>
+      </c>
+      <c r="G3" s="24">
         <f>F3-SUM(hours!G3:G6)</f>
-        <v>16.00</v>
-      </c>
-      <c r="H3" s="24" t="str">
+        <v>16</v>
+      </c>
+      <c r="H3" s="24">
         <f>G3-SUM(hours!H3:H6)</f>
-        <v>11.00</v>
-      </c>
-      <c r="I3" s="24" t="str">
+        <v>11</v>
+      </c>
+      <c r="I3" s="24">
         <f>H3-SUM(hours!I3:I6)</f>
-        <v>4.00</v>
+        <v>4</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2754,28 +4028,28 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>27</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
@@ -2783,39 +4057,39 @@
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="24" t="str">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <f>SUM(hours!B12:B15)</f>
-        <v>32.00</v>
-      </c>
-      <c r="C2" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="C2" s="24">
         <f>(B2/7)*6</f>
-        <v>27.43</v>
-      </c>
-      <c r="D2" s="24" t="str">
+        <v>27.42857143</v>
+      </c>
+      <c r="D2" s="24">
         <f>(B2/7)*5</f>
-        <v>22.86</v>
-      </c>
-      <c r="E2" s="24" t="str">
+        <v>22.85714286</v>
+      </c>
+      <c r="E2" s="24">
         <f>(B2/7)*4</f>
-        <v>18.29</v>
-      </c>
-      <c r="F2" s="24" t="str">
+        <v>18.28571429</v>
+      </c>
+      <c r="F2" s="24">
         <f>(B2/7)*3</f>
-        <v>13.71</v>
-      </c>
-      <c r="G2" s="24" t="str">
+        <v>13.71428571</v>
+      </c>
+      <c r="G2" s="24">
         <f>(B2/7)*2</f>
-        <v>9.14</v>
-      </c>
-      <c r="H2" s="24" t="str">
+        <v>9.142857143</v>
+      </c>
+      <c r="H2" s="24">
         <f>(B2/7)*1</f>
-        <v>4.57</v>
-      </c>
-      <c r="I2" s="24" t="str">
+        <v>4.571428571</v>
+      </c>
+      <c r="I2" s="24">
         <f>(B2/7)*0</f>
-        <v>0.00</v>
+        <v>0</v>
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
@@ -2823,42 +4097,42 @@
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
+        <f>B2</f>
+        <v>32</v>
+      </c>
+      <c r="C3" s="24">
+        <f>B3-SUM(hours!C12:C15)</f>
+        <v>20</v>
+      </c>
+      <c r="D3" s="24">
+        <f>C3-SUM(hours!D12:D15)</f>
+        <v>14</v>
+      </c>
+      <c r="E3" s="24">
+        <f>D3-SUM(hours!E12:E15)</f>
+        <v>14</v>
+      </c>
+      <c r="F3" s="24">
+        <f>E3-SUM(hours!F12:F15)</f>
+        <v>14</v>
+      </c>
+      <c r="G3" s="24">
+        <f>F3-SUM(hours!G12:G15)</f>
+        <v>8</v>
+      </c>
+      <c r="H3" s="24">
+        <f>G3-SUM(hours!H12:H15)</f>
+        <v>4</v>
+      </c>
+      <c r="I3" s="24">
+        <f>H3-SUM(hours!I12:I15)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="24" t="str">
-        <f>B2</f>
-        <v>32.00</v>
-      </c>
-      <c r="C3" s="24" t="str">
-        <f>B3-SUM(hours!C12:C15)</f>
-        <v>20.00</v>
-      </c>
-      <c r="D3" s="24" t="str">
-        <f>C3-SUM(hours!D12:D15)</f>
-        <v>14.00</v>
-      </c>
-      <c r="E3" s="24" t="str">
-        <f>D3-SUM(hours!E12:E15)</f>
-        <v>14.00</v>
-      </c>
-      <c r="F3" s="24" t="str">
-        <f>E3-SUM(hours!F12:F15)</f>
-        <v>14.00</v>
-      </c>
-      <c r="G3" s="24" t="str">
-        <f>F3-SUM(hours!G12:G15)</f>
-        <v>8.00</v>
-      </c>
-      <c r="H3" s="24" t="str">
-        <f>G3-SUM(hours!H12:H15)</f>
-        <v>4.00</v>
-      </c>
-      <c r="I3" s="24" t="str">
-        <f>H3-SUM(hours!I12:I15)</f>
-        <v>0.00</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
@@ -2897,189 +4171,189 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="J1" s="25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M1" s="25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="24" t="str">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <f>SUM(hours!B3:B6)+SUM(hours!B12:B15)</f>
-        <v>64.00</v>
-      </c>
-      <c r="C2" s="24" t="str">
+        <v>64</v>
+      </c>
+      <c r="C2" s="24">
         <f>(B2/14)*13</f>
-        <v>59.43</v>
-      </c>
-      <c r="D2" s="24" t="str">
+        <v>59.42857143</v>
+      </c>
+      <c r="D2" s="24">
         <f>(B2/14)*12</f>
-        <v>54.86</v>
-      </c>
-      <c r="E2" s="24" t="str">
+        <v>54.85714286</v>
+      </c>
+      <c r="E2" s="24">
         <f>(B2/14)*11</f>
-        <v>50.29</v>
-      </c>
-      <c r="F2" s="24" t="str">
+        <v>50.28571429</v>
+      </c>
+      <c r="F2" s="24">
         <f>(B2/14)*10</f>
-        <v>45.71</v>
-      </c>
-      <c r="G2" s="24" t="str">
+        <v>45.71428571</v>
+      </c>
+      <c r="G2" s="24">
         <f>(B2/14)*9</f>
-        <v>41.14</v>
-      </c>
-      <c r="H2" s="24" t="str">
+        <v>41.14285714</v>
+      </c>
+      <c r="H2" s="24">
         <f>(B2/14)*8</f>
-        <v>36.57</v>
-      </c>
-      <c r="I2" s="24" t="str">
+        <v>36.57142857</v>
+      </c>
+      <c r="I2" s="24">
         <f>(B2/14)*7</f>
-        <v>32.00</v>
-      </c>
-      <c r="J2" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="J2" s="24">
         <f>(B2/14)*6</f>
-        <v>27.43</v>
-      </c>
-      <c r="K2" s="24" t="str">
+        <v>27.42857143</v>
+      </c>
+      <c r="K2" s="24">
         <f>(B2/14)*5</f>
-        <v>22.86</v>
-      </c>
-      <c r="L2" s="24" t="str">
+        <v>22.85714286</v>
+      </c>
+      <c r="L2" s="24">
         <f>(B2/14)*4</f>
-        <v>18.29</v>
-      </c>
-      <c r="M2" s="24" t="str">
+        <v>18.28571429</v>
+      </c>
+      <c r="M2" s="24">
         <f>(B2/14)*3</f>
-        <v>13.71</v>
-      </c>
-      <c r="N2" s="24" t="str">
+        <v>13.71428571</v>
+      </c>
+      <c r="N2" s="24">
         <f>(B2/14)*2</f>
-        <v>9.14</v>
-      </c>
-      <c r="O2" s="24" t="str">
+        <v>9.142857143</v>
+      </c>
+      <c r="O2" s="24">
         <f>(B2/14)*1</f>
-        <v>4.57</v>
-      </c>
-      <c r="P2" s="24" t="str">
+        <v>4.571428571</v>
+      </c>
+      <c r="P2" s="24">
         <f>(B2/14)*0</f>
-        <v>0.00</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="24" t="str">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
         <f>B2</f>
-        <v>64.00</v>
-      </c>
-      <c r="C3" s="24" t="str">
+        <v>64</v>
+      </c>
+      <c r="C3" s="24">
         <f>B3-SUM(hours!C3:C6)</f>
-        <v>54.00</v>
-      </c>
-      <c r="D3" s="24" t="str">
+        <v>54</v>
+      </c>
+      <c r="D3" s="24">
         <f>C3-SUM(hours!D3:D6)</f>
-        <v>54.00</v>
-      </c>
-      <c r="E3" s="24" t="str">
+        <v>54</v>
+      </c>
+      <c r="E3" s="24">
         <f>D3-SUM(hours!E3:E6)</f>
-        <v>51.00</v>
-      </c>
-      <c r="F3" s="24" t="str">
+        <v>51</v>
+      </c>
+      <c r="F3" s="24">
         <f>E3-SUM(hours!F3:F6)</f>
-        <v>49.00</v>
-      </c>
-      <c r="G3" s="24" t="str">
+        <v>49</v>
+      </c>
+      <c r="G3" s="24">
         <f>F3-SUM(hours!G3:G6)</f>
-        <v>48.00</v>
-      </c>
-      <c r="H3" s="24" t="str">
+        <v>48</v>
+      </c>
+      <c r="H3" s="24">
         <f>G3-SUM(hours!H3:H6)</f>
-        <v>43.00</v>
-      </c>
-      <c r="I3" s="24" t="str">
+        <v>43</v>
+      </c>
+      <c r="I3" s="24">
         <f>H3-SUM(hours!I3:I6)</f>
-        <v>36.00</v>
-      </c>
-      <c r="J3" s="26" t="str">
+        <v>36</v>
+      </c>
+      <c r="J3" s="26">
         <f>I3-SUM(hours!C12:C15)</f>
-        <v>24.00</v>
-      </c>
-      <c r="K3" s="26" t="str">
+        <v>24</v>
+      </c>
+      <c r="K3" s="26">
         <f>J3-SUM(hours!D12:D15)</f>
-        <v>18.00</v>
-      </c>
-      <c r="L3" s="26" t="str">
+        <v>18</v>
+      </c>
+      <c r="L3" s="26">
         <f>K3-SUM(hours!E12:E15)</f>
-        <v>18.00</v>
-      </c>
-      <c r="M3" s="26" t="str">
+        <v>18</v>
+      </c>
+      <c r="M3" s="26">
         <f>L3-SUM(hours!F12:F15)</f>
-        <v>18.00</v>
-      </c>
-      <c r="N3" s="26" t="str">
+        <v>18</v>
+      </c>
+      <c r="N3" s="26">
         <f>M3-SUM(hours!G12:G15)</f>
-        <v>12.00</v>
-      </c>
-      <c r="O3" s="26" t="str">
+        <v>12</v>
+      </c>
+      <c r="O3" s="26">
         <f>N3-SUM(hours!H12:H15)</f>
-        <v>8.00</v>
-      </c>
-      <c r="P3" s="26" t="str">
+        <v>8</v>
+      </c>
+      <c r="P3" s="26">
         <f>O3-SUM(hours!I12:I15)</f>
-        <v>4.00</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="K8" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="K9" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3107,105 +4381,105 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="24" t="str">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <f>SUM(hours!B20:B23)</f>
-        <v>32.00</v>
-      </c>
-      <c r="C2" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="C2" s="24">
         <f>(B2/7)*6</f>
-        <v>27.43</v>
-      </c>
-      <c r="D2" s="24" t="str">
+        <v>27.42857143</v>
+      </c>
+      <c r="D2" s="24">
         <f>(B2/7)*5</f>
-        <v>22.86</v>
-      </c>
-      <c r="E2" s="24" t="str">
+        <v>22.85714286</v>
+      </c>
+      <c r="E2" s="24">
         <f>(B2/7)*4</f>
-        <v>18.29</v>
-      </c>
-      <c r="F2" s="24" t="str">
+        <v>18.28571429</v>
+      </c>
+      <c r="F2" s="24">
         <f>(B2/7)*3</f>
-        <v>13.71</v>
-      </c>
-      <c r="G2" s="24" t="str">
+        <v>13.71428571</v>
+      </c>
+      <c r="G2" s="24">
         <f>(B2/7)*2</f>
-        <v>9.14</v>
-      </c>
-      <c r="H2" s="24" t="str">
+        <v>9.142857143</v>
+      </c>
+      <c r="H2" s="24">
         <f>(B2/7)*1</f>
-        <v>4.57</v>
-      </c>
-      <c r="I2" s="24" t="str">
+        <v>4.571428571</v>
+      </c>
+      <c r="I2" s="24">
         <f>(B2/7)*0</f>
-        <v>0.00</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="24" t="str">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
         <f>B2</f>
-        <v>32.00</v>
-      </c>
-      <c r="C3" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="C3" s="24">
         <f>B3-SUM(hours!C20:C23)</f>
-        <v>21.00</v>
-      </c>
-      <c r="D3" s="24" t="str">
+        <v>21</v>
+      </c>
+      <c r="D3" s="24">
         <f>C3-SUM(hours!D20:D23)</f>
-        <v>19.00</v>
-      </c>
-      <c r="E3" s="24" t="str">
+        <v>19</v>
+      </c>
+      <c r="E3" s="24">
         <f>D3-SUM(hours!E20:E23)</f>
-        <v>18.00</v>
-      </c>
-      <c r="F3" s="24" t="str">
+        <v>18</v>
+      </c>
+      <c r="F3" s="24">
         <f>E3-SUM(hours!F20:F23)</f>
-        <v>15.00</v>
-      </c>
-      <c r="G3" s="24" t="str">
+        <v>15</v>
+      </c>
+      <c r="G3" s="24">
         <f>F3-SUM(hours!G20:G23)</f>
-        <v>13.00</v>
-      </c>
-      <c r="H3" s="24" t="str">
+        <v>13</v>
+      </c>
+      <c r="H3" s="24">
         <f>G3-SUM(hours!H20:H23)</f>
-        <v>6.00</v>
-      </c>
-      <c r="I3" s="24" t="str">
+        <v>6</v>
+      </c>
+      <c r="I3" s="24">
         <f>H3-SUM(hours!I20:I23)</f>
-        <v>4.00</v>
+        <v>4</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3235,105 +4509,105 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="24" t="str">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <f>SUM(hours!B28:B31)</f>
-        <v>32.00</v>
-      </c>
-      <c r="C2" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="C2" s="24">
         <f>(B2/7)*6</f>
-        <v>27.43</v>
-      </c>
-      <c r="D2" s="24" t="str">
+        <v>27.42857143</v>
+      </c>
+      <c r="D2" s="24">
         <f>(B2/7)*5</f>
-        <v>22.86</v>
-      </c>
-      <c r="E2" s="24" t="str">
+        <v>22.85714286</v>
+      </c>
+      <c r="E2" s="24">
         <f>(B2/7)*4</f>
-        <v>18.29</v>
-      </c>
-      <c r="F2" s="24" t="str">
+        <v>18.28571429</v>
+      </c>
+      <c r="F2" s="24">
         <f>(B2/7)*3</f>
-        <v>13.71</v>
-      </c>
-      <c r="G2" s="24" t="str">
+        <v>13.71428571</v>
+      </c>
+      <c r="G2" s="24">
         <f>(B2/7)*2</f>
-        <v>9.14</v>
-      </c>
-      <c r="H2" s="24" t="str">
+        <v>9.142857143</v>
+      </c>
+      <c r="H2" s="24">
         <f>(B2/7)*1</f>
-        <v>4.57</v>
-      </c>
-      <c r="I2" s="24" t="str">
+        <v>4.571428571</v>
+      </c>
+      <c r="I2" s="24">
         <f>(B2/7)*0</f>
-        <v>0.00</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="24" t="str">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
         <f>B2</f>
-        <v>32.00</v>
-      </c>
-      <c r="C3" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="C3" s="24">
         <f>B3-SUM(hours!C28:C31)</f>
-        <v>26.00</v>
-      </c>
-      <c r="D3" s="24" t="str">
+        <v>26</v>
+      </c>
+      <c r="D3" s="24">
         <f>C3-SUM(hours!D28:D31)</f>
-        <v>26.00</v>
-      </c>
-      <c r="E3" s="24" t="str">
+        <v>26</v>
+      </c>
+      <c r="E3" s="24">
         <f>D3-SUM(hours!E28:E31)</f>
-        <v>26.00</v>
-      </c>
-      <c r="F3" s="24" t="str">
+        <v>26</v>
+      </c>
+      <c r="F3" s="24">
         <f>E3-SUM(hours!F28:F31)</f>
-        <v>21.00</v>
-      </c>
-      <c r="G3" s="24" t="str">
+        <v>21</v>
+      </c>
+      <c r="G3" s="24">
         <f>F3-SUM(hours!G28:G31)</f>
-        <v>21.00</v>
-      </c>
-      <c r="H3" s="24" t="str">
+        <v>21</v>
+      </c>
+      <c r="H3" s="24">
         <f>G3-SUM(hours!H28:H31)</f>
-        <v>16.00</v>
-      </c>
-      <c r="I3" s="24" t="str">
+        <v>16</v>
+      </c>
+      <c r="I3" s="24">
         <f>H3-SUM(hours!I28:I31)</f>
-        <v>2.00</v>
+        <v>2</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3369,179 +4643,179 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="J1" s="25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M1" s="25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="24" t="str">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <f>SUM(hours!B20:B23)+SUM(hours!B28:B31)</f>
-        <v>64.00</v>
-      </c>
-      <c r="C2" s="24" t="str">
+        <v>64</v>
+      </c>
+      <c r="C2" s="24">
         <f>(B2/14)*13</f>
-        <v>59.43</v>
-      </c>
-      <c r="D2" s="24" t="str">
+        <v>59.42857143</v>
+      </c>
+      <c r="D2" s="24">
         <f>(B2/14)*12</f>
-        <v>54.86</v>
-      </c>
-      <c r="E2" s="24" t="str">
+        <v>54.85714286</v>
+      </c>
+      <c r="E2" s="24">
         <f>(B2/14)*11</f>
-        <v>50.29</v>
-      </c>
-      <c r="F2" s="24" t="str">
+        <v>50.28571429</v>
+      </c>
+      <c r="F2" s="24">
         <f>(B2/14)*10</f>
-        <v>45.71</v>
-      </c>
-      <c r="G2" s="24" t="str">
+        <v>45.71428571</v>
+      </c>
+      <c r="G2" s="24">
         <f>(B2/14)*9</f>
-        <v>41.14</v>
-      </c>
-      <c r="H2" s="24" t="str">
+        <v>41.14285714</v>
+      </c>
+      <c r="H2" s="24">
         <f>(B2/14)*8</f>
-        <v>36.57</v>
-      </c>
-      <c r="I2" s="24" t="str">
+        <v>36.57142857</v>
+      </c>
+      <c r="I2" s="24">
         <f>(B2/14)*7</f>
-        <v>32.00</v>
-      </c>
-      <c r="J2" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="J2" s="24">
         <f>(B2/14)*6</f>
-        <v>27.43</v>
-      </c>
-      <c r="K2" s="24" t="str">
+        <v>27.42857143</v>
+      </c>
+      <c r="K2" s="24">
         <f>(B2/14)*5</f>
-        <v>22.86</v>
-      </c>
-      <c r="L2" s="24" t="str">
+        <v>22.85714286</v>
+      </c>
+      <c r="L2" s="24">
         <f>(B2/14)*4</f>
-        <v>18.29</v>
-      </c>
-      <c r="M2" s="24" t="str">
+        <v>18.28571429</v>
+      </c>
+      <c r="M2" s="24">
         <f>(B2/14)*3</f>
-        <v>13.71</v>
-      </c>
-      <c r="N2" s="24" t="str">
+        <v>13.71428571</v>
+      </c>
+      <c r="N2" s="24">
         <f>(B2/14)*2</f>
-        <v>9.14</v>
-      </c>
-      <c r="O2" s="24" t="str">
+        <v>9.142857143</v>
+      </c>
+      <c r="O2" s="24">
         <f>(B2/14)*1</f>
-        <v>4.57</v>
-      </c>
-      <c r="P2" s="24" t="str">
+        <v>4.571428571</v>
+      </c>
+      <c r="P2" s="24">
         <f>(B2/14)*0</f>
-        <v>0.00</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
+        <f>B2</f>
+        <v>64</v>
+      </c>
+      <c r="C3" s="24">
+        <f>B3-SUM(hours!C20:C23)</f>
+        <v>53</v>
+      </c>
+      <c r="D3" s="24">
+        <f>C3-SUM(hours!D20:D23)</f>
+        <v>51</v>
+      </c>
+      <c r="E3" s="24">
+        <f>D3-SUM(hours!E20:E23)</f>
+        <v>50</v>
+      </c>
+      <c r="F3" s="24">
+        <f>E3-SUM(hours!F20:F23)</f>
+        <v>47</v>
+      </c>
+      <c r="G3" s="24">
+        <f>F3-SUM(hours!G20:G23)</f>
+        <v>45</v>
+      </c>
+      <c r="H3" s="24">
+        <f>G3-SUM(hours!H20:H23)</f>
+        <v>38</v>
+      </c>
+      <c r="I3" s="24">
+        <f>H3-SUM(hours!I20:I23)</f>
+        <v>36</v>
+      </c>
+      <c r="J3" s="26">
+        <f>I3-SUM(hours!C28:C31)</f>
         <v>30</v>
       </c>
-      <c r="B3" s="24" t="str">
-        <f>B2</f>
-        <v>64.00</v>
-      </c>
-      <c r="C3" s="24" t="str">
-        <f>B3-SUM(hours!C20:C23)</f>
-        <v>53.00</v>
-      </c>
-      <c r="D3" s="24" t="str">
-        <f>C3-SUM(hours!D20:D23)</f>
-        <v>51.00</v>
-      </c>
-      <c r="E3" s="24" t="str">
-        <f>D3-SUM(hours!E20:E23)</f>
-        <v>50.00</v>
-      </c>
-      <c r="F3" s="24" t="str">
-        <f>E3-SUM(hours!F20:F23)</f>
-        <v>47.00</v>
-      </c>
-      <c r="G3" s="24" t="str">
-        <f>F3-SUM(hours!G20:G23)</f>
-        <v>45.00</v>
-      </c>
-      <c r="H3" s="24" t="str">
-        <f>G3-SUM(hours!H20:H23)</f>
-        <v>38.00</v>
-      </c>
-      <c r="I3" s="24" t="str">
-        <f>H3-SUM(hours!I20:I23)</f>
-        <v>36.00</v>
-      </c>
-      <c r="J3" s="26" t="str">
-        <f>I3-SUM(hours!C28:C31)</f>
-        <v>30.00</v>
-      </c>
-      <c r="K3" s="26" t="str">
+      <c r="K3" s="26">
         <f>J3-SUM(hours!D28:D31)</f>
-        <v>30.00</v>
-      </c>
-      <c r="L3" s="26" t="str">
+        <v>30</v>
+      </c>
+      <c r="L3" s="26">
         <f>K3-SUM(hours!E28:E31)</f>
-        <v>30.00</v>
-      </c>
-      <c r="M3" s="26" t="str">
+        <v>30</v>
+      </c>
+      <c r="M3" s="26">
         <f>L3-SUM(hours!F28:F31)</f>
-        <v>25.00</v>
-      </c>
-      <c r="N3" s="26" t="str">
+        <v>25</v>
+      </c>
+      <c r="N3" s="26">
         <f>M3-SUM(hours!G28:G31)</f>
-        <v>25.00</v>
-      </c>
-      <c r="O3" s="26" t="str">
+        <v>25</v>
+      </c>
+      <c r="O3" s="26">
         <f>N3-SUM(hours!H28:H31)</f>
-        <v>20.00</v>
-      </c>
-      <c r="P3" s="26" t="str">
+        <v>20</v>
+      </c>
+      <c r="P3" s="26">
         <f>O3-SUM(hours!I28:I31)</f>
-        <v>6.00</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3592,338 +4866,460 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="J1" s="25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M1" s="25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="X1" s="25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y1" s="25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Z1" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA1" s="25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AB1" s="25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC1" s="25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AD1" s="25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="24" t="str">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <f>SUM(sprint1!B2)+SUM(sprint2!B2)</f>
-        <v>128.00</v>
-      </c>
-      <c r="C2" s="24" t="str">
+        <v>128</v>
+      </c>
+      <c r="C2" s="24">
         <f>(B2/28)*27</f>
-        <v>123.43</v>
-      </c>
-      <c r="D2" s="24" t="str">
+        <v>123.4285714</v>
+      </c>
+      <c r="D2" s="24">
         <f>(B2/28)*26</f>
-        <v>118.86</v>
-      </c>
-      <c r="E2" s="24" t="str">
+        <v>118.8571429</v>
+      </c>
+      <c r="E2" s="24">
         <f>((B2/28)*25)</f>
-        <v>114.29</v>
-      </c>
-      <c r="F2" s="24" t="str">
+        <v>114.2857143</v>
+      </c>
+      <c r="F2" s="24">
         <f>(B2/28)*24</f>
-        <v>109.71</v>
-      </c>
-      <c r="G2" s="24" t="str">
+        <v>109.7142857</v>
+      </c>
+      <c r="G2" s="24">
         <f>(B2/28)*23</f>
-        <v>105.14</v>
-      </c>
-      <c r="H2" s="24" t="str">
+        <v>105.1428571</v>
+      </c>
+      <c r="H2" s="24">
         <f>(B2/28)*22</f>
-        <v>100.57</v>
-      </c>
-      <c r="I2" s="24" t="str">
+        <v>100.5714286</v>
+      </c>
+      <c r="I2" s="24">
         <f>(B2/28)*21</f>
-        <v>96.00</v>
-      </c>
-      <c r="J2" s="24" t="str">
+        <v>96</v>
+      </c>
+      <c r="J2" s="24">
         <f>(B2/28)*20</f>
-        <v>91.43</v>
-      </c>
-      <c r="K2" s="24" t="str">
+        <v>91.42857143</v>
+      </c>
+      <c r="K2" s="24">
         <f>(B2/28)*19</f>
-        <v>86.86</v>
-      </c>
-      <c r="L2" s="24" t="str">
+        <v>86.85714286</v>
+      </c>
+      <c r="L2" s="24">
         <f>(B2/28)*18</f>
-        <v>82.29</v>
-      </c>
-      <c r="M2" s="24" t="str">
+        <v>82.28571429</v>
+      </c>
+      <c r="M2" s="24">
         <f>(B2/28)*17</f>
-        <v>77.71</v>
-      </c>
-      <c r="N2" s="24" t="str">
+        <v>77.71428571</v>
+      </c>
+      <c r="N2" s="24">
         <f>(B2/28)*16</f>
-        <v>73.14</v>
-      </c>
-      <c r="O2" s="24" t="str">
+        <v>73.14285714</v>
+      </c>
+      <c r="O2" s="24">
         <f>(B2/28)*15</f>
-        <v>68.57</v>
-      </c>
-      <c r="P2" s="24" t="str">
+        <v>68.57142857</v>
+      </c>
+      <c r="P2" s="24">
         <f>(B2/28)*14</f>
-        <v>64.00</v>
-      </c>
-      <c r="Q2" s="24" t="str">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="24">
         <f>(B2/28)*13</f>
-        <v>59.43</v>
-      </c>
-      <c r="R2" s="24" t="str">
+        <v>59.42857143</v>
+      </c>
+      <c r="R2" s="24">
         <f>(B2/28)*12</f>
-        <v>54.86</v>
-      </c>
-      <c r="S2" s="24" t="str">
+        <v>54.85714286</v>
+      </c>
+      <c r="S2" s="24">
         <f>(B2/28)*11</f>
-        <v>50.29</v>
-      </c>
-      <c r="T2" s="24" t="str">
+        <v>50.28571429</v>
+      </c>
+      <c r="T2" s="24">
         <f>(B2/28)*10</f>
-        <v>45.71</v>
-      </c>
-      <c r="U2" s="24" t="str">
+        <v>45.71428571</v>
+      </c>
+      <c r="U2" s="24">
         <f>(B2/28)*9</f>
-        <v>41.14</v>
-      </c>
-      <c r="V2" s="24" t="str">
+        <v>41.14285714</v>
+      </c>
+      <c r="V2" s="24">
         <f>(B2/28)*8</f>
-        <v>36.57</v>
-      </c>
-      <c r="W2" s="24" t="str">
+        <v>36.57142857</v>
+      </c>
+      <c r="W2" s="24">
         <f>(B2/28)*7</f>
-        <v>32.00</v>
-      </c>
-      <c r="X2" s="24" t="str">
+        <v>32</v>
+      </c>
+      <c r="X2" s="24">
         <f>(B2/28)*6</f>
-        <v>27.43</v>
-      </c>
-      <c r="Y2" s="24" t="str">
+        <v>27.42857143</v>
+      </c>
+      <c r="Y2" s="24">
         <f>(B2/28)*5</f>
-        <v>22.86</v>
-      </c>
-      <c r="Z2" s="24" t="str">
+        <v>22.85714286</v>
+      </c>
+      <c r="Z2" s="24">
         <f>(B2/28)*4</f>
-        <v>18.29</v>
-      </c>
-      <c r="AA2" s="24" t="str">
+        <v>18.28571429</v>
+      </c>
+      <c r="AA2" s="24">
         <f>(B2/28)*3</f>
-        <v>13.71</v>
-      </c>
-      <c r="AB2" s="24" t="str">
+        <v>13.71428571</v>
+      </c>
+      <c r="AB2" s="24">
         <f>(B2/28)*2</f>
-        <v>9.14</v>
-      </c>
-      <c r="AC2" s="24" t="str">
+        <v>9.142857143</v>
+      </c>
+      <c r="AC2" s="24">
         <f>(B2/28)*1</f>
-        <v>4.57</v>
-      </c>
-      <c r="AD2" s="24" t="str">
+        <v>4.571428571</v>
+      </c>
+      <c r="AD2" s="24">
         <f>(B2/28)*0</f>
-        <v>0.00</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="24" t="str">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
         <f>B2</f>
-        <v>128.00</v>
-      </c>
-      <c r="C3" s="24" t="str">
+        <v>128</v>
+      </c>
+      <c r="C3" s="24">
         <f>B3-SUM(hours!C3:C6)</f>
-        <v>118.00</v>
-      </c>
-      <c r="D3" s="24" t="str">
+        <v>118</v>
+      </c>
+      <c r="D3" s="24">
         <f>C3-SUM(hours!D3:D6)</f>
-        <v>118.00</v>
-      </c>
-      <c r="E3" s="24" t="str">
+        <v>118</v>
+      </c>
+      <c r="E3" s="24">
         <f>D3-SUM(hours!E3:E6)</f>
-        <v>115.00</v>
-      </c>
-      <c r="F3" s="24" t="str">
+        <v>115</v>
+      </c>
+      <c r="F3" s="24">
         <f>E3-SUM(hours!F3:F6)</f>
-        <v>113.00</v>
-      </c>
-      <c r="G3" s="24" t="str">
+        <v>113</v>
+      </c>
+      <c r="G3" s="24">
         <f>F3-SUM(hours!G3:G6)</f>
-        <v>112.00</v>
-      </c>
-      <c r="H3" s="24" t="str">
+        <v>112</v>
+      </c>
+      <c r="H3" s="24">
         <f>G3-SUM(hours!H3:H6)</f>
-        <v>107.00</v>
-      </c>
-      <c r="I3" s="24" t="str">
+        <v>107</v>
+      </c>
+      <c r="I3" s="24">
         <f>H3-SUM(hours!I3:I6)</f>
-        <v>100.00</v>
-      </c>
-      <c r="J3" s="24" t="str">
+        <v>100</v>
+      </c>
+      <c r="J3" s="24">
         <f>I3-SUM(hours!C12:C15)</f>
-        <v>88.00</v>
-      </c>
-      <c r="K3" s="24" t="str">
+        <v>88</v>
+      </c>
+      <c r="K3" s="24">
         <f>J3-SUM(hours!D12:D15)</f>
-        <v>82.00</v>
-      </c>
-      <c r="L3" s="24" t="str">
+        <v>82</v>
+      </c>
+      <c r="L3" s="24">
         <f>K3-SUM(hours!E12:E15)</f>
-        <v>82.00</v>
-      </c>
-      <c r="M3" s="24" t="str">
+        <v>82</v>
+      </c>
+      <c r="M3" s="24">
         <f>L3-SUM(hours!F12:F15)</f>
-        <v>82.00</v>
-      </c>
-      <c r="N3" s="24" t="str">
+        <v>82</v>
+      </c>
+      <c r="N3" s="24">
         <f>M3-SUM(hours!G12:G15)</f>
-        <v>76.00</v>
-      </c>
-      <c r="O3" s="24" t="str">
+        <v>76</v>
+      </c>
+      <c r="O3" s="24">
         <f>N3-SUM(hours!H12:H15)</f>
-        <v>72.00</v>
-      </c>
-      <c r="P3" s="24" t="str">
+        <v>72</v>
+      </c>
+      <c r="P3" s="24">
         <f>O3-SUM(hours!I12:I15)</f>
-        <v>68.00</v>
-      </c>
-      <c r="Q3" s="24" t="str">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="24">
         <f>P3-SUM(hours!C20:C23)</f>
-        <v>57.00</v>
-      </c>
-      <c r="R3" s="24" t="str">
+        <v>57</v>
+      </c>
+      <c r="R3" s="24">
         <f>Q3-SUM(hours!D20:D23)</f>
-        <v>55.00</v>
-      </c>
-      <c r="S3" s="24" t="str">
+        <v>55</v>
+      </c>
+      <c r="S3" s="24">
         <f>R3-SUM(hours!E20:E23)</f>
-        <v>54.00</v>
-      </c>
-      <c r="T3" s="24" t="str">
+        <v>54</v>
+      </c>
+      <c r="T3" s="24">
         <f>S3-SUM(hours!F20:F23)</f>
-        <v>51.00</v>
-      </c>
-      <c r="U3" s="24" t="str">
+        <v>51</v>
+      </c>
+      <c r="U3" s="24">
         <f>T3-SUM(hours!G20:G23)</f>
-        <v>49.00</v>
-      </c>
-      <c r="V3" s="24" t="str">
+        <v>49</v>
+      </c>
+      <c r="V3" s="24">
         <f>U3-SUM(hours!H20:H23)</f>
-        <v>42.00</v>
-      </c>
-      <c r="W3" s="24" t="str">
+        <v>42</v>
+      </c>
+      <c r="W3" s="24">
         <f>V3-SUM(hours!I20:I23)</f>
-        <v>40.00</v>
-      </c>
-      <c r="X3" s="26" t="str">
+        <v>40</v>
+      </c>
+      <c r="X3" s="26">
         <f>W3-SUM(hours!C28:C31)</f>
-        <v>34.00</v>
-      </c>
-      <c r="Y3" s="26" t="str">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="26">
         <f>X3-SUM(hours!D28:D31)</f>
-        <v>34.00</v>
-      </c>
-      <c r="Z3" s="26" t="str">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="26">
         <f>Y3-SUM(hours!E28:E31)</f>
-        <v>34.00</v>
-      </c>
-      <c r="AA3" s="26" t="str">
+        <v>34</v>
+      </c>
+      <c r="AA3" s="26">
         <f>Z3-SUM(hours!F28:F31)</f>
-        <v>29.00</v>
-      </c>
-      <c r="AB3" s="26" t="str">
+        <v>29</v>
+      </c>
+      <c r="AB3" s="26">
         <f>AA3-SUM(hours!G28:G31)</f>
-        <v>29.00</v>
-      </c>
-      <c r="AC3" s="26" t="str">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="26">
         <f>AB3-SUM(hours!H28:H31)</f>
-        <v>24.00</v>
-      </c>
-      <c r="AD3" s="26" t="str">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="26">
         <f>AC3-SUM(hours!I28:I31)</f>
-        <v>10.00</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="L6" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="21.14"/>
+    <col customWidth="1" min="3" max="4" width="10.0"/>
+    <col customWidth="1" min="5" max="5" width="8.86"/>
+    <col customWidth="1" min="6" max="6" width="9.71"/>
+    <col customWidth="1" min="7" max="7" width="10.0"/>
+    <col customWidth="1" min="8" max="8" width="10.57"/>
+    <col customWidth="1" min="9" max="9" width="9.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9"/>
+      <c r="B1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
+        <f>SUM(hours!B36:B39)</f>
+        <v>24</v>
+      </c>
+      <c r="C2" s="24">
+        <f>(B2/7)*6</f>
+        <v>20.57142857</v>
+      </c>
+      <c r="D2" s="24">
+        <f>(B2/7)*5</f>
+        <v>17.14285714</v>
+      </c>
+      <c r="E2" s="24">
+        <f>(B2/7)*4</f>
+        <v>13.71428571</v>
+      </c>
+      <c r="F2" s="24">
+        <f>(B2/7)*3</f>
+        <v>10.28571429</v>
+      </c>
+      <c r="G2" s="24">
+        <f>(B2/7)*2</f>
+        <v>6.857142857</v>
+      </c>
+      <c r="H2" s="24">
+        <f>(B2/7)*1</f>
+        <v>3.428571429</v>
+      </c>
+      <c r="I2" s="24">
+        <f>(B2/7)*0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24">
+        <f>B2</f>
+        <v>24</v>
+      </c>
+      <c r="C3" s="24">
+        <f>B3-SUM(hours!C36:C39)</f>
+        <v>13</v>
+      </c>
+      <c r="D3" s="24">
+        <f>C3-SUM(hours!D36:D39)</f>
+        <v>13</v>
+      </c>
+      <c r="E3" s="24">
+        <f>D3-SUM(hours!E36:E39)</f>
+        <v>11</v>
+      </c>
+      <c r="F3" s="24">
+        <f>E3-SUM(hours!F36:F39)</f>
+        <v>7</v>
+      </c>
+      <c r="G3" s="24">
+        <f>F3-SUM(hours!G36:G39)</f>
+        <v>5</v>
+      </c>
+      <c r="H3" s="24">
+        <f>G3-SUM(hours!H36:H39)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="24">
+        <f>H3-SUM(hours!I36:I39)</f>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>